<commit_message>
Se crearon los servicios, modelos y main script para Codigo de Red
</commit_message>
<xml_diff>
--- a/input/Tabla 4 - Datos Medición.xlsx
+++ b/input/Tabla 4 - Datos Medición.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ae599aac914ac79b/Desktop/VSCodeProyectos/Python/MVP_InnovaPQ/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_9D30839260D13BC4E3D0B1B4DEC910655E02D804" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8FF20053-DE16-4A4A-BBBD-D96BFA9C5E64}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_9D30839260D13BC4E3D0B1B4DEC910655E02D804" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69567BB5-02FE-4D2D-83E0-60BDC2BD9C68}"/>
   <bookViews>
-    <workbookView xWindow="20415" yWindow="3510" windowWidth="16680" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="16680" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -133,6 +133,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -338,11 +342,13 @@
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" customWidth="1"/>
+    <col min="1" max="1" width="42.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>